<commit_message>
edit in Stock on Hand + Finish From Land
</commit_message>
<xml_diff>
--- a/Stock on Hands/Layouts/StockOnHand.xlsx
+++ b/Stock on Hands/Layouts/StockOnHand.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\BC-Projects\Stock on hand\Layouts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\BC-Projects\Stock on Hands\Layouts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A5A90B-44F2-4AD7-B0A3-1E05670B95CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2E0273-1981-4982-988E-2AECFBC5D578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -188,6 +188,9 @@
     <t>Description</t>
   </si>
   <si>
+    <t>BaseUnit</t>
+  </si>
+  <si>
     <t>Unit_Cost</t>
   </si>
   <si>
@@ -207,9 +210,6 @@
   </si>
   <si>
     <t>Total_Consumption</t>
-  </si>
-  <si>
-    <t>BaseUnit</t>
   </si>
   <si>
     <t>Gen_Prod_Posting_Group</t>
@@ -234,7 +234,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
@@ -248,14 +248,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Amasis MT Pro Light"/>
-      <family val="1"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,6 +259,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC0C0C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -281,29 +281,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="عادي" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="5">
     <dxf>
       <font>
         <b/>
@@ -315,68 +303,19 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color auto="1"/>
-        <name val="Amasis MT Pro Light"/>
-        <family val="1"/>
-        <scheme val="none"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFC0C0C0"/>
+          <bgColor theme="0" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -492,26 +431,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" name="Data" displayName="Data" ref="A1:O2" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" name="Data" displayName="Data" ref="A1:O2" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:O2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Item_No" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Description" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Unit_Cost" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Stock_On_Hand" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Total_Cost" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Quantity_Purchases" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Total_Purchases" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Quantity_Consumed" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Total_Consumption" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BaseUnit" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Gen_Prod_Posting_Group" dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Item_Catogry" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Location_Code" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="StartDate" dataDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="EndDate" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Item_No"/>
+    <tableColumn id="2" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Description"/>
+    <tableColumn id="3" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BaseUnit"/>
+    <tableColumn id="4" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Unit_Cost"/>
+    <tableColumn id="5" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Stock_On_Hand"/>
+    <tableColumn id="6" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Total_Cost"/>
+    <tableColumn id="7" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Quantity_Purchases"/>
+    <tableColumn id="8" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Total_Purchases"/>
+    <tableColumn id="9" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Quantity_Consumed"/>
+    <tableColumn id="10" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Total_Consumption"/>
+    <tableColumn id="11" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Gen_Prod_Posting_Group"/>
+    <tableColumn id="12" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Item_Catogry"/>
+    <tableColumn id="13" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Location_Code"/>
+    <tableColumn id="14" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="StartDate"/>
+    <tableColumn id="15" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="EndDate"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -539,7 +478,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{134EB915-8B19-4838-BDED-CECBACACF4F9}" name="ReportMetadataValues" displayName="ReportMetadataValues" ref="A1:B10" totalsRowShown="0" headerRowDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{134EB915-8B19-4838-BDED-CECBACACF4F9}" name="ReportMetadataValues" displayName="ReportMetadataValues" ref="A1:B10" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:B10" xr:uid="{134EB915-8B19-4838-BDED-CECBACACF4F9}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{5CBC1C08-5A8D-42BB-92CA-C3F1D0EF0A4D}" name="Report Property"/>
@@ -550,7 +489,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{1DFF5EE2-2A86-40DE-9DFD-1E96553323F6}" name="ReportRequestValues" displayName="ReportRequestValues" ref="D1:E10" totalsRowShown="0" headerRowDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{1DFF5EE2-2A86-40DE-9DFD-1E96553323F6}" name="ReportRequestValues" displayName="ReportRequestValues" ref="D1:E10" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="D1:E10" xr:uid="{1DFF5EE2-2A86-40DE-9DFD-1E96553323F6}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{E6EF2D44-8AB2-42E8-A7E3-9B148922AA59}" name="Request Property"/>
@@ -561,7 +500,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8D3A40BA-47FA-41F3-82A4-C5BD4909C0B4}" name="ReportRequestPageValues" displayName="ReportRequestPageValues" ref="G1:H2" totalsRowShown="0" headerRowDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8D3A40BA-47FA-41F3-82A4-C5BD4909C0B4}" name="ReportRequestPageValues" displayName="ReportRequestPageValues" ref="G1:H2" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="G1:H2" xr:uid="{8D3A40BA-47FA-41F3-82A4-C5BD4909C0B4}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{023648B2-C225-4580-B767-C48467418032}" name="Request Page Option"/>
@@ -572,7 +511,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D269260C-C433-478B-84A3-3CB73C333872}" name="ReportFilterValues" displayName="ReportFilterValues" ref="J1:K2" totalsRowShown="0" headerRowDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D269260C-C433-478B-84A3-3CB73C333872}" name="ReportFilterValues" displayName="ReportFilterValues" ref="J1:K2" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="J1:K2" xr:uid="{D269260C-C433-478B-84A3-3CB73C333872}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{D710F0AA-F8F4-4DB2-BC43-E65C2054A321}" name="Filter"/>
@@ -879,124 +818,123 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.8984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.09765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.8984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.09765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.59765625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.69921875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.69921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.09765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.8984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.09765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="P1" s="2"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="2">
         <v>0</v>
       </c>
-      <c r="D2" s="4">
+      <c r="E2" s="2">
         <v>0</v>
       </c>
-      <c r="E2" s="4">
+      <c r="F2" s="2">
         <v>0</v>
       </c>
-      <c r="F2" s="4">
+      <c r="G2" s="2">
         <v>0</v>
       </c>
-      <c r="G2" s="4">
+      <c r="H2" s="2">
         <v>0</v>
       </c>
-      <c r="H2" s="4">
+      <c r="I2" s="2">
         <v>0</v>
       </c>
-      <c r="I2" s="4">
+      <c r="J2" s="2">
         <v>0</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" t="s">
         <v>63</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" t="s">
         <v>63</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" t="s">
         <v>63</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="N2" s="5">
+      <c r="N2" s="3">
         <v>0</v>
       </c>
-      <c r="O2" s="5">
+      <c r="O2" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>